<commit_message>
Teste de conteúdo das colunas agora leva em consideração equivalencia com substituição de espaços por underscore e de caracteres especiais
</commit_message>
<xml_diff>
--- a/Template - Relatório de teste.xlsx
+++ b/Template - Relatório de teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/lucas_rocha2_br_ey_com/Documents/Documents/Chubb/comparaTabelasCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{A5802189-6F34-47B2-BD01-C7D2D92662C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9F618AF-CF2B-48CC-A6E0-62719DF66869}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{A5802189-6F34-47B2-BD01-C7D2D92662C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36FB86A2-0561-4BE9-815D-8D42EC0E09DC}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{850903C5-D053-47AF-9BE4-30F0F3D838BC}"/>
+    <workbookView xWindow="46584" yWindow="7296" windowWidth="21600" windowHeight="11388" xr2:uid="{850903C5-D053-47AF-9BE4-30F0F3D838BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -269,12 +269,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -636,7 +630,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,67 +644,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -750,10 +744,10 @@
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -763,10 +757,10 @@
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,10 +770,10 @@
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -789,10 +783,10 @@
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -802,10 +796,10 @@
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -815,10 +809,10 @@
       <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -828,10 +822,10 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -841,10 +835,10 @@
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -854,10 +848,10 @@
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -867,10 +861,10 @@
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>